<commit_message>
update return dict and create getVersion()
</commit_message>
<xml_diff>
--- a/Interface web/exemple_liste.xlsx
+++ b/Interface web/exemple_liste.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FLE\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ecambxl-my.sharepoint.com/personal/17076_ecam_be/Documents/Ecole/Master 1/Q2/Projet Robot/KorreKthor/Interface web/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_4086817CFE8FC2D621F05A6516DF56A869228FBC" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_4086817CFE8FC2D621F05A6516DF56A869228FBC" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8D320404-A15F-4F50-B824-257FB2DCFD79}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="34">
   <si>
     <t>cotes_2021_4eisd40_juin</t>
   </si>
@@ -118,13 +118,28 @@
   </si>
   <si>
     <t>VANDERMIES Charles</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -133,6 +148,17 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -155,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -165,6 +191,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,25 +473,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1"/>
     <col min="3" max="3" width="54" customWidth="1"/>
     <col min="4" max="4" width="6" customWidth="1"/>
-    <col min="5" max="5" width="44.5703125" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="44.59765625" customWidth="1"/>
+    <col min="6" max="6" width="6.73046875" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" customWidth="1"/>
+    <col min="8" max="8" width="8.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -475,7 +503,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -500,8 +528,11 @@
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -518,8 +549,11 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -536,8 +570,11 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -554,8 +591,11 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -572,8 +612,11 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -590,8 +633,11 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -608,8 +654,11 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -626,8 +675,11 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -644,8 +696,11 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -662,8 +717,11 @@
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
       <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
@@ -680,8 +738,11 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
@@ -698,8 +759,11 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
@@ -716,8 +780,11 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="4" t="s">
         <v>12</v>
       </c>
@@ -734,8 +801,11 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
@@ -752,8 +822,11 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="I16" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
@@ -767,8 +840,11 @@
       <c r="E17" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="I17" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="4" t="s">
         <v>12</v>
       </c>
@@ -781,6 +857,9 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
         <v>11</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -788,19 +867,11 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008363491AB45800439C60E5A4AFEEFD7B" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="bd968deeac1585f8dce456b69f03d27c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9a086da1-f6b6-4775-9bed-6a1f1d23dd5e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="03b8d306141823516372461e3a3187c9" ns2:_="">
     <xsd:import namespace="9a086da1-f6b6-4775-9bed-6a1f1d23dd5e"/>
@@ -932,6 +1003,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -939,13 +1019,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB8E40AD-9265-40D6-9AF2-9D7659819022}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DC8E71B-4498-481C-B008-0BDAE5EBCBF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9a086da1-f6b6-4775-9bed-6a1f1d23dd5e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DC8E71B-4498-481C-B008-0BDAE5EBCBF4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB8E40AD-9265-40D6-9AF2-9D7659819022}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C0AB5F2-35DE-410C-B519-5BD2E467F978}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C0AB5F2-35DE-410C-B519-5BD2E467F978}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>